<commit_message>
allows userse to upload either csv or xlsx for the custom layout
</commit_message>
<xml_diff>
--- a/data-raw/2024-use-case/2024 JPE Events 3+4 Files + Plating Scheme v5 (1)/030124_JPE24_EL_E3-4_P1_SH_v2.xlsx
+++ b/data-raw/2024-use-case/2024 JPE Events 3+4 Files + Plating Scheme v5 (1)/030124_JPE24_EL_E3-4_P1_SH_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canfi\OneDrive\Desktop\GVL-DWR_Stuff\JPE\2024\Results\SHERLOCK\E3+4\Ots28\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuel\projects\jpe\grunID\data-raw\2024-use-case\2024 JPE Events 3+4 Files + Plating Scheme v5 (1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C633AEFB-12F7-4330-B245-6009CC41A109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CD908D-B964-4E35-BE2A-D1653120D5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sherlock_output" sheetId="1" r:id="rId1"/>
@@ -1768,9 +1768,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1808,7 +1808,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1914,7 +1914,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2056,7 +2056,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2066,17 +2066,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:CU295"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="AC137" sqref="AC137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>0.42865740740740743</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>21111913</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2148,13 +2148,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2162,12 +2162,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2175,12 +2175,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2196,53 +2196,53 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="6">
         <v>1</v>
@@ -2317,7 +2317,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>35</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>54</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>55</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>74</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>75</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>94</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>95</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>114</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>117</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>138</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>141</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>160</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>163</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>182</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>183</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>200</v>
       </c>
@@ -3157,13 +3157,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>484530</v>
       </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="51" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:99" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>9</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="52" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B52" s="12">
         <v>0</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="53" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B53" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="54" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B54" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="55" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B55" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>2445</v>
       </c>
     </row>
-    <row r="56" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B56" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>2720</v>
       </c>
     </row>
-    <row r="57" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B57" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>2926</v>
       </c>
     </row>
-    <row r="58" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B58" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="59" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B59" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="60" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B60" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>3263</v>
       </c>
     </row>
-    <row r="61" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B61" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="62" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B62" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>3407</v>
       </c>
     </row>
-    <row r="63" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B63" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>3553</v>
       </c>
     </row>
-    <row r="64" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B64" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>3478</v>
       </c>
     </row>
-    <row r="65" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B65" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>3604</v>
       </c>
     </row>
-    <row r="66" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B66" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>3715</v>
       </c>
     </row>
-    <row r="67" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B67" s="12">
         <v>3.125E-2</v>
       </c>
@@ -8195,7 +8195,7 @@
         <v>3691</v>
       </c>
     </row>
-    <row r="68" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B68" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>3804</v>
       </c>
     </row>
-    <row r="69" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B69" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>3823</v>
       </c>
     </row>
-    <row r="70" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B70" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>3820</v>
       </c>
     </row>
-    <row r="71" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B71" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>4044</v>
       </c>
     </row>
-    <row r="72" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B72" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>3981</v>
       </c>
     </row>
-    <row r="73" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B73" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>4084</v>
       </c>
     </row>
-    <row r="74" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B74" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -10267,7 +10267,7 @@
         <v>4074</v>
       </c>
     </row>
-    <row r="75" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B75" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="76" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B76" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>4103</v>
       </c>
     </row>
-    <row r="77" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B77" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -11155,7 +11155,7 @@
         <v>4203</v>
       </c>
     </row>
-    <row r="78" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B78" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>4253</v>
       </c>
     </row>
-    <row r="79" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B79" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>4274</v>
       </c>
     </row>
-    <row r="80" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B80" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -12043,7 +12043,7 @@
         <v>4378</v>
       </c>
     </row>
-    <row r="81" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B81" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>4462</v>
       </c>
     </row>
-    <row r="82" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B82" s="12">
         <v>6.25E-2</v>
       </c>
@@ -12635,7 +12635,7 @@
         <v>4487</v>
       </c>
     </row>
-    <row r="83" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B83" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -12931,7 +12931,7 @@
         <v>4505</v>
       </c>
     </row>
-    <row r="84" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B84" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -13227,7 +13227,7 @@
         <v>4470</v>
       </c>
     </row>
-    <row r="85" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B85" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -13523,7 +13523,7 @@
         <v>4521</v>
       </c>
     </row>
-    <row r="86" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B86" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -13819,7 +13819,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="87" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B87" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -14115,7 +14115,7 @@
         <v>4664</v>
       </c>
     </row>
-    <row r="88" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B88" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>4551</v>
       </c>
     </row>
-    <row r="89" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B89" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -14707,7 +14707,7 @@
         <v>4701</v>
       </c>
     </row>
-    <row r="90" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B90" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -15003,7 +15003,7 @@
         <v>4708</v>
       </c>
     </row>
-    <row r="91" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B91" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15299,7 +15299,7 @@
         <v>4759</v>
       </c>
     </row>
-    <row r="92" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B92" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -15595,13 +15595,13 @@
         <v>4730</v>
       </c>
     </row>
-    <row r="94" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <v>484530</v>
       </c>
       <c r="B94" s="4"/>
     </row>
-    <row r="96" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:99" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B96" s="6" t="s">
         <v>9</v>
       </c>
@@ -15813,7 +15813,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="97" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B97" s="12">
         <v>0</v>
       </c>
@@ -16025,7 +16025,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="98" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B98" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -16237,7 +16237,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="99" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B99" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -16449,7 +16449,7 @@
         <v>2852</v>
       </c>
     </row>
-    <row r="100" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B100" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -16661,7 +16661,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="101" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B101" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -16873,7 +16873,7 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="102" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B102" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -17085,7 +17085,7 @@
         <v>3770</v>
       </c>
     </row>
-    <row r="103" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B103" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -17297,7 +17297,7 @@
         <v>3824</v>
       </c>
     </row>
-    <row r="104" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B104" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -17509,7 +17509,7 @@
         <v>4030</v>
       </c>
     </row>
-    <row r="105" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B105" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -17721,7 +17721,7 @@
         <v>4194</v>
       </c>
     </row>
-    <row r="106" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B106" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -17933,7 +17933,7 @@
         <v>4242</v>
       </c>
     </row>
-    <row r="107" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B107" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -18145,7 +18145,7 @@
         <v>4390</v>
       </c>
     </row>
-    <row r="108" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B108" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -18357,7 +18357,7 @@
         <v>4497</v>
       </c>
     </row>
-    <row r="109" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B109" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -18569,7 +18569,7 @@
         <v>4516</v>
       </c>
     </row>
-    <row r="110" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B110" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -18781,7 +18781,7 @@
         <v>4717</v>
       </c>
     </row>
-    <row r="111" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B111" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -18993,7 +18993,7 @@
         <v>4684</v>
       </c>
     </row>
-    <row r="112" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B112" s="12">
         <v>3.125E-2</v>
       </c>
@@ -19205,7 +19205,7 @@
         <v>4729</v>
       </c>
     </row>
-    <row r="113" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B113" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -19417,7 +19417,7 @@
         <v>4922</v>
       </c>
     </row>
-    <row r="114" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B114" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -19629,7 +19629,7 @@
         <v>4904</v>
       </c>
     </row>
-    <row r="115" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B115" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -19841,7 +19841,7 @@
         <v>4987</v>
       </c>
     </row>
-    <row r="116" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B116" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -20053,7 +20053,7 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="117" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B117" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -20265,7 +20265,7 @@
         <v>5037</v>
       </c>
     </row>
-    <row r="118" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B118" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -20477,7 +20477,7 @@
         <v>5106</v>
       </c>
     </row>
-    <row r="119" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B119" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -20689,7 +20689,7 @@
         <v>5173</v>
       </c>
     </row>
-    <row r="120" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B120" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -20901,7 +20901,7 @@
         <v>5130</v>
       </c>
     </row>
-    <row r="121" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B121" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -21113,7 +21113,7 @@
         <v>5255</v>
       </c>
     </row>
-    <row r="122" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B122" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -21325,7 +21325,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="123" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B123" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -21537,7 +21537,7 @@
         <v>5259</v>
       </c>
     </row>
-    <row r="124" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B124" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -21749,7 +21749,7 @@
         <v>5438</v>
       </c>
     </row>
-    <row r="125" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B125" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -21961,7 +21961,7 @@
         <v>5484</v>
       </c>
     </row>
-    <row r="126" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B126" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -22173,7 +22173,7 @@
         <v>5287</v>
       </c>
     </row>
-    <row r="127" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B127" s="12">
         <v>6.25E-2</v>
       </c>
@@ -22385,7 +22385,7 @@
         <v>5493</v>
       </c>
     </row>
-    <row r="128" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:71" x14ac:dyDescent="0.25">
       <c r="B128" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -22597,7 +22597,7 @@
         <v>5654</v>
       </c>
     </row>
-    <row r="129" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B129" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -22809,7 +22809,7 @@
         <v>5610</v>
       </c>
     </row>
-    <row r="130" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B130" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -23021,7 +23021,7 @@
         <v>5638</v>
       </c>
     </row>
-    <row r="131" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B131" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -23233,7 +23233,7 @@
         <v>5512</v>
       </c>
     </row>
-    <row r="132" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B132" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -23445,7 +23445,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="133" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B133" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -23657,7 +23657,7 @@
         <v>5702</v>
       </c>
     </row>
-    <row r="134" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B134" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -23869,7 +23869,7 @@
         <v>5789</v>
       </c>
     </row>
-    <row r="135" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B135" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -24081,7 +24081,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="136" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B136" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -24293,7 +24293,7 @@
         <v>5927</v>
       </c>
     </row>
-    <row r="137" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B137" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -24505,13 +24505,13 @@
         <v>5930</v>
       </c>
     </row>
-    <row r="139" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>366</v>
       </c>
       <c r="B139" s="4"/>
     </row>
-    <row r="141" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B141" s="6" t="s">
         <v>9</v>
       </c>
@@ -24804,7 +24804,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="142" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B142" s="12">
         <v>0</v>
       </c>
@@ -25097,7 +25097,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="143" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B143" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -25390,7 +25390,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="144" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B144" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -25683,7 +25683,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="145" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B145" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -25976,7 +25976,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="146" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B146" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -26269,7 +26269,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="147" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B147" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -26562,7 +26562,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="148" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B148" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -26855,7 +26855,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="149" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B149" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -27148,7 +27148,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="150" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B150" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -27441,7 +27441,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="151" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B151" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -27734,7 +27734,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="152" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B152" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -28027,7 +28027,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="153" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B153" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -28320,7 +28320,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="154" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B154" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -28613,7 +28613,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="155" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B155" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -28906,7 +28906,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="156" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B156" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -29199,7 +29199,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="157" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B157" s="12">
         <v>3.125E-2</v>
       </c>
@@ -29492,7 +29492,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="158" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B158" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -29785,7 +29785,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="159" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B159" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -30078,7 +30078,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="160" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B160" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -30371,7 +30371,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="161" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B161" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -30664,7 +30664,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="162" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B162" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -30957,7 +30957,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="163" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B163" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -31250,7 +31250,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="164" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B164" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -31543,7 +31543,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="165" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B165" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -31836,7 +31836,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="166" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B166" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -32129,7 +32129,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="167" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B167" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -32422,7 +32422,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="168" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B168" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -32715,7 +32715,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="169" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B169" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -33008,7 +33008,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="170" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B170" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -33301,7 +33301,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="171" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B171" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -33594,7 +33594,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="172" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B172" s="12">
         <v>6.25E-2</v>
       </c>
@@ -33887,7 +33887,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="173" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B173" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -34180,7 +34180,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="174" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B174" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -34473,7 +34473,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="175" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B175" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -34766,7 +34766,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="176" spans="2:98" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:98" x14ac:dyDescent="0.25">
       <c r="B176" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -35059,7 +35059,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="177" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B177" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -35352,7 +35352,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="178" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B178" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -35645,7 +35645,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="179" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B179" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -35938,7 +35938,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="180" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B180" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -36231,7 +36231,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="181" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B181" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -36524,7 +36524,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="182" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B182" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -36817,13 +36817,13 @@
         <v>448</v>
       </c>
     </row>
-    <row r="184" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>366</v>
       </c>
       <c r="B184" s="4"/>
     </row>
-    <row r="186" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B186" s="6" t="s">
         <v>9</v>
       </c>
@@ -37032,7 +37032,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="187" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B187" s="12">
         <v>0</v>
       </c>
@@ -37241,7 +37241,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="188" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B188" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -37450,7 +37450,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="189" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B189" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -37659,7 +37659,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="190" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B190" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -37868,7 +37868,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="191" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B191" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -38077,7 +38077,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="192" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B192" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -38286,7 +38286,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="193" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B193" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -38495,7 +38495,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="194" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B194" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -38704,7 +38704,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="195" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B195" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -38913,7 +38913,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="196" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B196" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -39122,7 +39122,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="197" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B197" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -39331,7 +39331,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="198" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B198" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -39540,7 +39540,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="199" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B199" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -39749,7 +39749,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="200" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B200" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -39958,7 +39958,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="201" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B201" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -40167,7 +40167,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="202" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B202" s="12">
         <v>3.125E-2</v>
       </c>
@@ -40376,7 +40376,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="203" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B203" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -40585,7 +40585,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="204" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B204" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -40794,7 +40794,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="205" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B205" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -41003,7 +41003,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="206" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B206" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -41212,7 +41212,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="207" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B207" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -41421,7 +41421,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="208" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B208" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -41630,7 +41630,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="209" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B209" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -41839,7 +41839,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="210" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B210" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -42048,7 +42048,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="211" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B211" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -42257,7 +42257,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="212" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B212" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -42466,7 +42466,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="213" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B213" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -42675,7 +42675,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="214" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B214" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -42884,7 +42884,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="215" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B215" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -43093,7 +43093,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="216" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B216" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -43302,7 +43302,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="217" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B217" s="12">
         <v>6.25E-2</v>
       </c>
@@ -43511,7 +43511,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="218" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B218" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -43720,7 +43720,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="219" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B219" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -43929,7 +43929,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="220" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B220" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -44138,7 +44138,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="221" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B221" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -44347,7 +44347,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="222" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B222" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -44556,7 +44556,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="223" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B223" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -44765,7 +44765,7 @@
         <v>1551</v>
       </c>
     </row>
-    <row r="224" spans="2:70" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B224" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -44974,7 +44974,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="225" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B225" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -45183,7 +45183,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="226" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B226" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -45392,7 +45392,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="227" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B227" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -45601,13 +45601,13 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="229" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B229" s="4"/>
     </row>
-    <row r="231" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B231" s="5"/>
       <c r="C231" s="6">
         <v>1</v>
@@ -45682,7 +45682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="232" spans="1:70" ht="18" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:70" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B232" s="32" t="s">
         <v>35</v>
       </c>
@@ -45754,7 +45754,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="233" spans="1:70" ht="27" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:70" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B233" s="33"/>
       <c r="C233" s="15">
         <v>0.999</v>
@@ -45824,7 +45824,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="234" spans="1:70" ht="27" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:70" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B234" s="33"/>
       <c r="C234" s="16">
         <v>1.8749999999999999E-2</v>
@@ -45894,7 +45894,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="235" spans="1:70" ht="27" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:70" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B235" s="34"/>
       <c r="C235" s="17">
         <v>1.306712962962963E-2</v>
@@ -45964,7 +45964,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="236" spans="1:70" ht="18" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:70" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B236" s="32" t="s">
         <v>54</v>
       </c>
@@ -45996,7 +45996,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="237" spans="1:70" ht="27" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:70" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B237" s="33"/>
       <c r="C237" s="15"/>
       <c r="D237" s="15"/>
@@ -46026,7 +46026,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="238" spans="1:70" ht="27" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:70" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B238" s="33"/>
       <c r="C238" s="15"/>
       <c r="D238" s="15"/>
@@ -46056,7 +46056,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="239" spans="1:70" ht="27" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:70" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B239" s="34"/>
       <c r="C239" s="18"/>
       <c r="D239" s="18"/>
@@ -46086,7 +46086,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="240" spans="1:70" ht="18" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:70" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B240" s="32" t="s">
         <v>55</v>
       </c>
@@ -46158,7 +46158,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="241" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B241" s="33"/>
       <c r="C241" s="15">
         <v>0.97899999999999998</v>
@@ -46228,7 +46228,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="242" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B242" s="33"/>
       <c r="C242" s="16">
         <v>1.6666666666666666E-2</v>
@@ -46298,7 +46298,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="243" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B243" s="34"/>
       <c r="C243" s="17">
         <v>1.1736111111111109E-2</v>
@@ -46368,7 +46368,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="244" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B244" s="32" t="s">
         <v>74</v>
       </c>
@@ -46400,7 +46400,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="245" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B245" s="33"/>
       <c r="C245" s="15"/>
       <c r="D245" s="15"/>
@@ -46430,7 +46430,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="246" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B246" s="33"/>
       <c r="C246" s="15"/>
       <c r="D246" s="15"/>
@@ -46460,7 +46460,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="247" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B247" s="34"/>
       <c r="C247" s="18"/>
       <c r="D247" s="18"/>
@@ -46490,7 +46490,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="248" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B248" s="32" t="s">
         <v>75</v>
       </c>
@@ -46562,7 +46562,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="249" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B249" s="33"/>
       <c r="C249" s="15">
         <v>0.98299999999999998</v>
@@ -46632,7 +46632,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="250" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B250" s="33"/>
       <c r="C250" s="16">
         <v>1.6666666666666666E-2</v>
@@ -46702,7 +46702,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="251" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B251" s="34"/>
       <c r="C251" s="17">
         <v>1.1990740740740739E-2</v>
@@ -46772,7 +46772,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="252" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B252" s="32" t="s">
         <v>94</v>
       </c>
@@ -46804,7 +46804,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="253" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B253" s="33"/>
       <c r="C253" s="15"/>
       <c r="D253" s="15"/>
@@ -46834,7 +46834,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="254" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B254" s="33"/>
       <c r="C254" s="15"/>
       <c r="D254" s="15"/>
@@ -46864,7 +46864,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="255" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B255" s="34"/>
       <c r="C255" s="18"/>
       <c r="D255" s="18"/>
@@ -46894,7 +46894,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="256" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B256" s="32" t="s">
         <v>95</v>
       </c>
@@ -46966,7 +46966,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="257" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B257" s="33"/>
       <c r="C257" s="15">
         <v>0.98699999999999999</v>
@@ -47036,7 +47036,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="258" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B258" s="33"/>
       <c r="C258" s="16">
         <v>1.6666666666666666E-2</v>
@@ -47106,7 +47106,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="259" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B259" s="34"/>
       <c r="C259" s="17">
         <v>1.2893518518518519E-2</v>
@@ -47176,7 +47176,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="260" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B260" s="32" t="s">
         <v>114</v>
       </c>
@@ -47212,7 +47212,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="261" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B261" s="33"/>
       <c r="C261" s="15"/>
       <c r="D261" s="15"/>
@@ -47246,7 +47246,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="262" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B262" s="33"/>
       <c r="C262" s="15"/>
       <c r="D262" s="15"/>
@@ -47280,7 +47280,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="263" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B263" s="34"/>
       <c r="C263" s="18"/>
       <c r="D263" s="18"/>
@@ -47314,7 +47314,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="264" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B264" s="32" t="s">
         <v>117</v>
       </c>
@@ -47386,7 +47386,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="265" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B265" s="33"/>
       <c r="C265" s="15">
         <v>0.97499999999999998</v>
@@ -47456,7 +47456,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="266" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B266" s="33"/>
       <c r="C266" s="16">
         <v>1.6666666666666666E-2</v>
@@ -47526,7 +47526,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="267" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B267" s="34"/>
       <c r="C267" s="17">
         <v>1.2361111111111113E-2</v>
@@ -47596,7 +47596,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="268" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B268" s="32" t="s">
         <v>138</v>
       </c>
@@ -47632,7 +47632,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="269" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B269" s="33"/>
       <c r="C269" s="15"/>
       <c r="D269" s="15"/>
@@ -47666,7 +47666,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="270" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B270" s="33"/>
       <c r="C270" s="15"/>
       <c r="D270" s="15"/>
@@ -47700,7 +47700,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="271" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B271" s="34"/>
       <c r="C271" s="18"/>
       <c r="D271" s="18"/>
@@ -47734,7 +47734,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="272" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B272" s="32" t="s">
         <v>141</v>
       </c>
@@ -47802,7 +47802,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="273" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B273" s="33"/>
       <c r="C273" s="15">
         <v>0.97</v>
@@ -47868,7 +47868,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="274" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B274" s="33"/>
       <c r="C274" s="16">
         <v>1.6666666666666666E-2</v>
@@ -47934,7 +47934,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="275" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B275" s="34"/>
       <c r="C275" s="17">
         <v>1.2314814814814815E-2</v>
@@ -48000,7 +48000,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="276" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B276" s="32" t="s">
         <v>160</v>
       </c>
@@ -48036,7 +48036,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="277" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B277" s="33"/>
       <c r="C277" s="15"/>
       <c r="D277" s="15"/>
@@ -48070,7 +48070,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="278" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B278" s="33"/>
       <c r="C278" s="15"/>
       <c r="D278" s="15"/>
@@ -48104,7 +48104,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="279" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B279" s="34"/>
       <c r="C279" s="18"/>
       <c r="D279" s="18"/>
@@ -48138,7 +48138,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="280" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B280" s="32" t="s">
         <v>163</v>
       </c>
@@ -48206,7 +48206,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="281" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B281" s="33"/>
       <c r="C281" s="15">
         <v>0.98499999999999999</v>
@@ -48272,7 +48272,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="282" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B282" s="33"/>
       <c r="C282" s="16">
         <v>1.6666666666666666E-2</v>
@@ -48338,7 +48338,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="283" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B283" s="34"/>
       <c r="C283" s="17">
         <v>1.2488425925925925E-2</v>
@@ -48404,7 +48404,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="284" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B284" s="32" t="s">
         <v>182</v>
       </c>
@@ -48440,7 +48440,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="285" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B285" s="33"/>
       <c r="C285" s="15"/>
       <c r="D285" s="15"/>
@@ -48474,7 +48474,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="286" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B286" s="33"/>
       <c r="C286" s="15"/>
       <c r="D286" s="15"/>
@@ -48508,7 +48508,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="287" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B287" s="34"/>
       <c r="C287" s="18"/>
       <c r="D287" s="18"/>
@@ -48542,7 +48542,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="288" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B288" s="32" t="s">
         <v>183</v>
       </c>
@@ -48610,7 +48610,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="289" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B289" s="33"/>
       <c r="C289" s="15">
         <v>0.98399999999999999</v>
@@ -48676,7 +48676,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="290" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B290" s="33"/>
       <c r="C290" s="16">
         <v>1.6666666666666666E-2</v>
@@ -48742,7 +48742,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="291" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B291" s="34"/>
       <c r="C291" s="17">
         <v>1.2268518518518519E-2</v>
@@ -48808,7 +48808,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="292" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B292" s="32" t="s">
         <v>200</v>
       </c>
@@ -48844,7 +48844,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="293" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B293" s="33"/>
       <c r="C293" s="15"/>
       <c r="D293" s="15"/>
@@ -48878,7 +48878,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="294" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B294" s="33"/>
       <c r="C294" s="15"/>
       <c r="D294" s="15"/>
@@ -48912,7 +48912,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="295" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B295" s="34"/>
       <c r="C295" s="18"/>
       <c r="D295" s="18"/>
@@ -48948,11 +48948,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B232:B235"/>
-    <mergeCell ref="B236:B239"/>
-    <mergeCell ref="B240:B243"/>
-    <mergeCell ref="B244:B247"/>
-    <mergeCell ref="B248:B251"/>
     <mergeCell ref="B252:B255"/>
     <mergeCell ref="B280:B283"/>
     <mergeCell ref="B284:B287"/>
@@ -48964,6 +48959,11 @@
     <mergeCell ref="B268:B271"/>
     <mergeCell ref="B272:B275"/>
     <mergeCell ref="B276:B279"/>
+    <mergeCell ref="B232:B235"/>
+    <mergeCell ref="B236:B239"/>
+    <mergeCell ref="B240:B243"/>
+    <mergeCell ref="B244:B247"/>
+    <mergeCell ref="B248:B251"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -48975,17 +48975,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1E8B86-B84B-44B8-A11C-91B182E5EA2E}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="25" width="15.85546875" customWidth="1"/>
+    <col min="2" max="25" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19">
         <v>1</v>
       </c>
@@ -49059,7 +49059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>35</v>
       </c>
@@ -49128,7 +49128,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>54</v>
       </c>
@@ -49157,7 +49157,7 @@
       <c r="X3" s="23"/>
       <c r="Y3" s="24"/>
     </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>55</v>
       </c>
@@ -49226,7 +49226,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>74</v>
       </c>
@@ -49255,7 +49255,7 @@
       <c r="X5" s="23"/>
       <c r="Y5" s="24"/>
     </row>
-    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>75</v>
       </c>
@@ -49324,7 +49324,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>94</v>
       </c>
@@ -49353,7 +49353,7 @@
       <c r="X7" s="23"/>
       <c r="Y7" s="24"/>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>95</v>
       </c>
@@ -49422,7 +49422,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>114</v>
       </c>
@@ -49455,7 +49455,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>117</v>
       </c>
@@ -49524,7 +49524,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>138</v>
       </c>
@@ -49557,7 +49557,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>141</v>
       </c>
@@ -49622,7 +49622,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>160</v>
       </c>
@@ -49655,7 +49655,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>163</v>
       </c>
@@ -49720,7 +49720,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>182</v>
       </c>
@@ -49753,7 +49753,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>183</v>
       </c>
@@ -49818,7 +49818,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>200</v>
       </c>
@@ -49851,7 +49851,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="N18" s="31"/>
     </row>
   </sheetData>
@@ -49860,24 +49860,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a707c639-4ab7-466f-ab80-9083af4ef22b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7" xsi:nil="true"/>
-    <SharedWithUsers xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009AE391E1779C514D98B0AAF78991A34A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20865b83f50b8ce2b19f31cddc80d719">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a707c639-4ab7-466f-ab80-9083af4ef22b" xmlns:ns3="02ee1384-56f9-49a7-aa58-df62156adfc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0acb1623640e290c6f9e9b40375a9f1" ns2:_="" ns3:_="">
     <xsd:import namespace="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
@@ -50106,6 +50088,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a707c639-4ab7-466f-ab80-9083af4ef22b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7" xsi:nil="true"/>
+    <SharedWithUsers xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -50116,17 +50116,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{572AB6E5-9620-471B-8E73-D218E983FA15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
-    <ds:schemaRef ds:uri="02ee1384-56f9-49a7-aa58-df62156adfc7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50E8F17E-0077-4E1C-9940-B3121635721C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50145,6 +50134,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{572AB6E5-9620-471B-8E73-D218E983FA15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
+    <ds:schemaRef ds:uri="02ee1384-56f9-49a7-aa58-df62156adfc7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF9DB72D-6BBB-44FF-A8FD-81C499D85B4B}">
   <ds:schemaRefs>

</xml_diff>